<commit_message>
ID 5860834302 - Attendees initial
Updated the attendees initials fields comments
</commit_message>
<xml_diff>
--- a/02_Beta/IWR V1.10.xlsx
+++ b/02_Beta/IWR V1.10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Shared\Z_DevCyntech\KZS\06_IWR\03_Beta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A Dev\kzs-tkt-2106-IWR\02_Beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04A2C49-50E2-4B03-8123-6FCC28BC5DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3802CF-EB12-4781-BE1E-F76EAE6EB295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,32 +43,33 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={4F92BA45-3C49-4D81-B0C9-D64F50403ACE}</author>
-    <author>tc={E8A35062-D7EF-41B2-BB01-2AD50C91D7E0}</author>
+    <author>tc={3E2E70C1-362C-4ECB-8A31-7D04567DE348}</author>
+    <author>tc={68747DDA-9089-4F4A-8123-58FD6A81BD3F}</author>
     <author>tc={9C5DE710-6CCD-4CBC-A02F-0457CA86E66B}</author>
-    <author>tc={E5A7CF71-D59B-4525-A1CC-7FF69AB1FE8D}</author>
-    <author>tc={DAC5AFE6-EDD5-4AB4-A046-10DDF16F13AC}</author>
-    <author>tc={2B2067F4-67AF-40A7-8CA0-51D148C7FF3C}</author>
+    <author>tc={ABB743D8-7036-4343-806A-FE99DB464625}</author>
+    <author>tc={C25A2B51-F298-470B-932B-1BD9B5FFACCE}</author>
+    <author>tc={A4BE263C-8657-4FC6-A725-70B24A834954}</author>
     <author>tc={901122A2-B3CA-4C30-9216-F14785E9FC09}</author>
     <author>tc={B9D4DAD7-E3F2-4616-9808-F4DDAB33766F}</author>
   </authors>
   <commentList>
-    <comment ref="G123" authorId="0" shapeId="0" xr:uid="{4F92BA45-3C49-4D81-B0C9-D64F50403ACE}">
+    <comment ref="G123" authorId="0" shapeId="0" xr:uid="{3E2E70C1-362C-4ECB-8A31-7D04567DE348}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    CYU: David J. 
-CYL: Tyler B.</t>
+    CYU: David J.
+CYL: Jon L.</t>
       </text>
     </comment>
-    <comment ref="N123" authorId="1" shapeId="0" xr:uid="{E8A35062-D7EF-41B2-BB01-2AD50C91D7E0}">
+    <comment ref="N123" authorId="1" shapeId="0" xr:uid="{68747DDA-9089-4F4A-8123-58FD6A81BD3F}">
       <text>
-        <t>[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    CYU: Brian W.
-CYL: Dustin W.</t>
+    CYU: Dustin W.
+CYL: Ryan B.
+</t>
       </text>
     </comment>
     <comment ref="B124" authorId="2" shapeId="0" xr:uid="{9C5DE710-6CCD-4CBC-A02F-0457CA86E66B}">
@@ -80,30 +81,31 @@
 CYL: Joe P.</t>
       </text>
     </comment>
-    <comment ref="G124" authorId="3" shapeId="0" xr:uid="{E5A7CF71-D59B-4525-A1CC-7FF69AB1FE8D}">
+    <comment ref="G124" authorId="3" shapeId="0" xr:uid="{ABB743D8-7036-4343-806A-FE99DB464625}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    CYU: Jennifer B. 
+CYL: Jennifer B, Jon L. 
+</t>
+      </text>
+    </comment>
+    <comment ref="N124" authorId="4" shapeId="0" xr:uid="{C25A2B51-F298-470B-932B-1BD9B5FFACCE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    CYU: Shawn F. 
-CYL: Tyler B.</t>
+    CYU/CYL: David B, Cameron M.</t>
       </text>
     </comment>
-    <comment ref="N124" authorId="4" shapeId="0" xr:uid="{DAC5AFE6-EDD5-4AB4-A046-10DDF16F13AC}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    CYU/CYL: David B.</t>
-      </text>
-    </comment>
-    <comment ref="B125" authorId="5" shapeId="0" xr:uid="{2B2067F4-67AF-40A7-8CA0-51D148C7FF3C}">
+    <comment ref="B125" authorId="5" shapeId="0" xr:uid="{A4BE263C-8657-4FC6-A725-70B24A834954}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     CYU: Donny H.
-CYL: Tyler B.</t>
+CYL: Jon L.</t>
       </text>
     </comment>
     <comment ref="G125" authorId="6" shapeId="0" xr:uid="{901122A2-B3CA-4C30-9216-F14785E9FC09}">
@@ -603,15 +605,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="00000"/>
-    <numFmt numFmtId="167" formatCode="#,##0&quot; lbs&quot;"/>
-    <numFmt numFmtId="168" formatCode="#,##0&quot; hrs&quot;"/>
-    <numFmt numFmtId="169" formatCode="0."/>
-    <numFmt numFmtId="170" formatCode="#,##0.0&quot; wks&quot;"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="00000"/>
+    <numFmt numFmtId="166" formatCode="#,##0&quot; lbs&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0&quot; hrs&quot;"/>
+    <numFmt numFmtId="168" formatCode="0."/>
+    <numFmt numFmtId="169" formatCode="#,##0.0&quot; wks&quot;"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -802,6 +804,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1226,7 +1234,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1295,7 +1303,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1387,13 +1395,331 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="17" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="17" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="17" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1403,324 +1729,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="17" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="17" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="17" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1803,6 +1811,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Sossa, Melany" id="{6FC8C94A-ABBA-4DCC-99FF-1425B5779617}" userId="S::Melany.sossa@cyntechgroup.com::808d24b1-bbd0-4d88-b522-67be7bbad099" providerId="AD"/>
   <person displayName="Hindbo, Brandon" id="{D4ADA3FA-577E-4235-B12E-1D0A931E021F}" userId="S::Brandon.Hindbo@cyntechgroup.com::45e31011-3334-4393-b605-379339653f78" providerId="AD"/>
   <person displayName="Hindbo, Brandon" id="{ED934490-859F-4E76-8750-054F90A275CD}" userId="S::Brandon.Hindbo@cyntechgroup.com::a6afa42a-31de-4f86-a4af-768925395489" providerId="AD"/>
 </personList>
@@ -2095,28 +2104,30 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G123" dT="2021-12-23T20:46:04.02" personId="{ED934490-859F-4E76-8750-054F90A275CD}" id="{4F92BA45-3C49-4D81-B0C9-D64F50403ACE}">
-    <text>CYU: David J. 
-CYL: Tyler B.</text>
+  <threadedComment ref="G123" dT="2024-01-15T23:51:46.43" personId="{6FC8C94A-ABBA-4DCC-99FF-1425B5779617}" id="{3E2E70C1-362C-4ECB-8A31-7D04567DE348}">
+    <text>CYU: David J.
+CYL: Jon L.</text>
   </threadedComment>
-  <threadedComment ref="N123" dT="2022-05-19T21:55:07.05" personId="{ED934490-859F-4E76-8750-054F90A275CD}" id="{E8A35062-D7EF-41B2-BB01-2AD50C91D7E0}">
-    <text>CYU: Brian W.
-CYL: Dustin W.</text>
+  <threadedComment ref="N123" dT="2024-01-15T23:53:32.01" personId="{6FC8C94A-ABBA-4DCC-99FF-1425B5779617}" id="{68747DDA-9089-4F4A-8123-58FD6A81BD3F}">
+    <text xml:space="preserve">CYU: Dustin W.
+CYL: Ryan B.
+</text>
   </threadedComment>
   <threadedComment ref="B124" dT="2022-05-19T21:53:59.73" personId="{ED934490-859F-4E76-8750-054F90A275CD}" id="{9C5DE710-6CCD-4CBC-A02F-0457CA86E66B}">
     <text>CYU: Allan B, Donnie T., or both
 CYL: Joe P.</text>
   </threadedComment>
-  <threadedComment ref="G124" dT="2021-12-23T20:46:04.02" personId="{ED934490-859F-4E76-8750-054F90A275CD}" id="{E5A7CF71-D59B-4525-A1CC-7FF69AB1FE8D}">
-    <text>CYU: Shawn F. 
-CYL: Tyler B.</text>
+  <threadedComment ref="G124" dT="2024-01-15T23:52:42.93" personId="{6FC8C94A-ABBA-4DCC-99FF-1425B5779617}" id="{ABB743D8-7036-4343-806A-FE99DB464625}">
+    <text xml:space="preserve">CYU: Jennifer B. 
+CYL: Jennifer B, Jon L. 
+</text>
   </threadedComment>
-  <threadedComment ref="N124" dT="2021-04-23T15:57:45.20" personId="{D4ADA3FA-577E-4235-B12E-1D0A931E021F}" id="{DAC5AFE6-EDD5-4AB4-A046-10DDF16F13AC}">
-    <text>CYU/CYL: David B.</text>
+  <threadedComment ref="N124" dT="2024-01-15T23:53:50.55" personId="{6FC8C94A-ABBA-4DCC-99FF-1425B5779617}" id="{C25A2B51-F298-470B-932B-1BD9B5FFACCE}">
+    <text>CYU/CYL: David B, Cameron M.</text>
   </threadedComment>
-  <threadedComment ref="B125" dT="2022-05-19T21:56:29.49" personId="{ED934490-859F-4E76-8750-054F90A275CD}" id="{2B2067F4-67AF-40A7-8CA0-51D148C7FF3C}">
+  <threadedComment ref="B125" dT="2024-01-15T23:51:07.15" personId="{6FC8C94A-ABBA-4DCC-99FF-1425B5779617}" id="{A4BE263C-8657-4FC6-A725-70B24A834954}">
     <text>CYU: Donny H.
-CYL: Tyler B.</text>
+CYL: Jon L.</text>
   </threadedComment>
   <threadedComment ref="G125" dT="2021-04-23T15:54:59.96" personId="{D4ADA3FA-577E-4235-B12E-1D0A931E021F}" id="{901122A2-B3CA-4C30-9216-F14785E9FC09}">
     <text>CYU/CYL: Zach B.</text>
@@ -2131,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF179"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7:Q8"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageBreakPreview" topLeftCell="A109" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L135" sqref="L135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2173,11 +2184,11 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -2185,21 +2196,21 @@
     </row>
     <row r="2" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
-      <c r="P2" s="115"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
@@ -2228,19 +2239,19 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
+      <c r="I4" s="118"/>
+      <c r="J4" s="118"/>
+      <c r="K4" s="118"/>
+      <c r="L4" s="118"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="53" t="s">
+      <c r="N4" s="101" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="56"/>
+      <c r="O4" s="114"/>
+      <c r="P4" s="114"/>
+      <c r="Q4" s="115"/>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2251,17 +2262,17 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="118"/>
+      <c r="K5" s="118"/>
+      <c r="L5" s="118"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="58"/>
+      <c r="N5" s="103"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="116"/>
+      <c r="Q5" s="117"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2272,12 +2283,12 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
       <c r="M6" s="1"/>
       <c r="R6" s="1"/>
     </row>
@@ -2289,24 +2300,24 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="119" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="119"/>
+      <c r="J7" s="119"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="53" t="s">
+      <c r="N7" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="O7" s="65"/>
-      <c r="P7" s="55">
+      <c r="O7" s="102"/>
+      <c r="P7" s="114">
         <f>ROUND((G14-G12)/7,1)</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="56"/>
+      <c r="Q7" s="115"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2317,17 +2328,17 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="57"/>
-      <c r="Q8" s="58"/>
+      <c r="N8" s="103"/>
+      <c r="O8" s="104"/>
+      <c r="P8" s="116"/>
+      <c r="Q8" s="117"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2365,14 +2376,14 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="53" t="s">
+      <c r="N10" s="101" t="s">
         <v>42</v>
       </c>
-      <c r="O10" s="65"/>
-      <c r="P10" s="67">
+      <c r="O10" s="102"/>
+      <c r="P10" s="124">
         <v>0</v>
       </c>
-      <c r="Q10" s="68"/>
+      <c r="Q10" s="125"/>
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2383,19 +2394,19 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="G11" s="129"/>
-      <c r="H11" s="129"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
       <c r="I11"/>
-      <c r="J11" s="72" t="s">
+      <c r="J11" s="128" t="s">
         <v>92</v>
       </c>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72"/>
+      <c r="K11" s="128"/>
+      <c r="L11" s="128"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="66"/>
-      <c r="P11" s="69"/>
-      <c r="Q11" s="70"/>
+      <c r="N11" s="103"/>
+      <c r="O11" s="104"/>
+      <c r="P11" s="126"/>
+      <c r="Q11" s="127"/>
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2406,12 +2417,12 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
+      <c r="G12" s="93"/>
+      <c r="H12" s="93"/>
       <c r="I12"/>
-      <c r="J12" s="72"/>
-      <c r="K12" s="72"/>
-      <c r="L12" s="72"/>
+      <c r="J12" s="128"/>
+      <c r="K12" s="128"/>
+      <c r="L12" s="128"/>
       <c r="M12" s="1"/>
       <c r="R12" s="1"/>
     </row>
@@ -2423,22 +2434,22 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
+      <c r="G13" s="93"/>
+      <c r="H13" s="93"/>
       <c r="I13"/>
-      <c r="J13" s="72"/>
-      <c r="K13" s="72"/>
-      <c r="L13" s="72"/>
+      <c r="J13" s="128"/>
+      <c r="K13" s="128"/>
+      <c r="L13" s="128"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="53" t="s">
+      <c r="N13" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="O13" s="65"/>
-      <c r="P13" s="61">
+      <c r="O13" s="102"/>
+      <c r="P13" s="120">
         <f>SUMPRODUCT(O20:O43,C20:C43)</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="62"/>
+      <c r="Q13" s="121"/>
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2449,17 +2460,17 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
+      <c r="G14" s="93"/>
+      <c r="H14" s="93"/>
       <c r="I14"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="72"/>
-      <c r="L14" s="72"/>
+      <c r="J14" s="128"/>
+      <c r="K14" s="128"/>
+      <c r="L14" s="128"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="66"/>
-      <c r="P14" s="63"/>
-      <c r="Q14" s="64"/>
+      <c r="N14" s="103"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="122"/>
+      <c r="Q14" s="123"/>
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2532,28 +2543,28 @@
     </row>
     <row r="18" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="81" t="s">
+      <c r="B18" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="81" t="s">
+      <c r="C18" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="116" t="s">
+      <c r="D18" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="117"/>
-      <c r="F18" s="99" t="s">
+      <c r="E18" s="58"/>
+      <c r="F18" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="100"/>
-      <c r="H18" s="100"/>
-      <c r="I18" s="100"/>
-      <c r="J18" s="100"/>
-      <c r="K18" s="100"/>
-      <c r="L18" s="100"/>
-      <c r="M18" s="100"/>
-      <c r="N18" s="122"/>
-      <c r="O18" s="81" t="s">
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="70"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="70"/>
+      <c r="M18" s="70"/>
+      <c r="N18" s="71"/>
+      <c r="O18" s="97" t="s">
         <v>46</v>
       </c>
       <c r="P18" s="84" t="s">
@@ -2566,20 +2577,20 @@
     </row>
     <row r="19" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="118"/>
-      <c r="E19" s="119"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="102"/>
-      <c r="I19" s="102"/>
-      <c r="J19" s="102"/>
-      <c r="K19" s="102"/>
-      <c r="L19" s="102"/>
-      <c r="M19" s="102"/>
-      <c r="N19" s="123"/>
-      <c r="O19" s="82"/>
+      <c r="B19" s="98"/>
+      <c r="C19" s="98"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="73"/>
+      <c r="L19" s="73"/>
+      <c r="M19" s="73"/>
+      <c r="N19" s="74"/>
+      <c r="O19" s="98"/>
       <c r="P19" s="86"/>
       <c r="Q19" s="87"/>
       <c r="R19" s="1"/>
@@ -2588,552 +2599,552 @@
     </row>
     <row r="20" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="77">
+      <c r="B20" s="54">
         <v>1</v>
       </c>
-      <c r="C20" s="79">
+      <c r="C20" s="94">
         <v>99</v>
       </c>
-      <c r="D20" s="120">
+      <c r="D20" s="61">
         <v>999</v>
       </c>
-      <c r="E20" s="121"/>
-      <c r="F20" s="124" t="s">
+      <c r="E20" s="62"/>
+      <c r="F20" s="75" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="125"/>
-      <c r="H20" s="125"/>
-      <c r="I20" s="125"/>
-      <c r="J20" s="125"/>
-      <c r="K20" s="125"/>
-      <c r="L20" s="125"/>
-      <c r="M20" s="125"/>
-      <c r="N20" s="126"/>
-      <c r="O20" s="130"/>
-      <c r="P20" s="127"/>
-      <c r="Q20" s="128"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="76"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="77"/>
+      <c r="O20" s="99"/>
+      <c r="P20" s="88"/>
+      <c r="Q20" s="89"/>
       <c r="R20" s="1"/>
       <c r="AE20"/>
       <c r="AF20"/>
     </row>
     <row r="21" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="77"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="96"/>
-      <c r="F21" s="105" t="s">
+      <c r="B21" s="54"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="106"/>
-      <c r="J21" s="106"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="106"/>
-      <c r="M21" s="106"/>
-      <c r="N21" s="107"/>
-      <c r="O21" s="113"/>
-      <c r="P21" s="74"/>
-      <c r="Q21" s="75"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="79"/>
+      <c r="J21" s="79"/>
+      <c r="K21" s="79"/>
+      <c r="L21" s="79"/>
+      <c r="M21" s="79"/>
+      <c r="N21" s="80"/>
+      <c r="O21" s="100"/>
+      <c r="P21" s="90"/>
+      <c r="Q21" s="91"/>
       <c r="R21" s="1"/>
       <c r="AE21"/>
       <c r="AF21"/>
     </row>
     <row r="22" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="78"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="108"/>
-      <c r="G22" s="109"/>
-      <c r="H22" s="109"/>
-      <c r="I22" s="109"/>
-      <c r="J22" s="109"/>
-      <c r="K22" s="109"/>
-      <c r="L22" s="109"/>
-      <c r="M22" s="109"/>
-      <c r="N22" s="110"/>
-      <c r="O22" s="113"/>
-      <c r="P22" s="74"/>
-      <c r="Q22" s="75"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="81"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="83"/>
+      <c r="O22" s="100"/>
+      <c r="P22" s="90"/>
+      <c r="Q22" s="91"/>
       <c r="R22" s="1"/>
       <c r="AE22"/>
       <c r="AF22"/>
     </row>
     <row r="23" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="83">
+      <c r="B23" s="56">
         <v>2</v>
       </c>
-      <c r="C23" s="92"/>
-      <c r="D23" s="93"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="106"/>
-      <c r="H23" s="106"/>
-      <c r="I23" s="106"/>
-      <c r="J23" s="106"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="106"/>
-      <c r="N23" s="107"/>
-      <c r="O23" s="113"/>
-      <c r="P23" s="74"/>
-      <c r="Q23" s="75"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="78"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="80"/>
+      <c r="O23" s="100"/>
+      <c r="P23" s="90"/>
+      <c r="Q23" s="91"/>
       <c r="R23" s="1"/>
       <c r="AE23"/>
       <c r="AF23"/>
     </row>
     <row r="24" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="77"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="106"/>
-      <c r="H24" s="106"/>
-      <c r="I24" s="106"/>
-      <c r="J24" s="106"/>
-      <c r="K24" s="106"/>
-      <c r="L24" s="106"/>
-      <c r="M24" s="106"/>
-      <c r="N24" s="107"/>
-      <c r="O24" s="113"/>
-      <c r="P24" s="74"/>
-      <c r="Q24" s="75"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="78"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="79"/>
+      <c r="J24" s="79"/>
+      <c r="K24" s="79"/>
+      <c r="L24" s="79"/>
+      <c r="M24" s="79"/>
+      <c r="N24" s="80"/>
+      <c r="O24" s="100"/>
+      <c r="P24" s="90"/>
+      <c r="Q24" s="91"/>
       <c r="R24" s="1"/>
       <c r="AE24"/>
       <c r="AF24"/>
     </row>
     <row r="25" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="78"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="97"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="108"/>
-      <c r="G25" s="109"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="109"/>
-      <c r="J25" s="109"/>
-      <c r="K25" s="109"/>
-      <c r="L25" s="109"/>
-      <c r="M25" s="109"/>
-      <c r="N25" s="110"/>
-      <c r="O25" s="113"/>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="75"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="82"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="82"/>
+      <c r="L25" s="82"/>
+      <c r="M25" s="82"/>
+      <c r="N25" s="83"/>
+      <c r="O25" s="100"/>
+      <c r="P25" s="90"/>
+      <c r="Q25" s="91"/>
       <c r="R25" s="1"/>
       <c r="AE25"/>
       <c r="AF25"/>
     </row>
     <row r="26" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="83">
+      <c r="B26" s="56">
         <v>3</v>
       </c>
-      <c r="C26" s="92"/>
-      <c r="D26" s="93"/>
-      <c r="E26" s="94"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="106"/>
-      <c r="H26" s="106"/>
-      <c r="I26" s="106"/>
-      <c r="J26" s="106"/>
-      <c r="K26" s="106"/>
-      <c r="L26" s="106"/>
-      <c r="M26" s="106"/>
-      <c r="N26" s="107"/>
-      <c r="O26" s="113"/>
-      <c r="P26" s="74"/>
-      <c r="Q26" s="75"/>
+      <c r="C26" s="96"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="79"/>
+      <c r="J26" s="79"/>
+      <c r="K26" s="79"/>
+      <c r="L26" s="79"/>
+      <c r="M26" s="79"/>
+      <c r="N26" s="80"/>
+      <c r="O26" s="100"/>
+      <c r="P26" s="90"/>
+      <c r="Q26" s="91"/>
       <c r="R26" s="1"/>
       <c r="AE26"/>
       <c r="AF26"/>
     </row>
     <row r="27" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="79"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="96"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="106"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="106"/>
-      <c r="K27" s="106"/>
-      <c r="L27" s="106"/>
-      <c r="M27" s="106"/>
-      <c r="N27" s="107"/>
-      <c r="O27" s="113"/>
-      <c r="P27" s="74"/>
-      <c r="Q27" s="75"/>
+      <c r="B27" s="54"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="79"/>
+      <c r="J27" s="79"/>
+      <c r="K27" s="79"/>
+      <c r="L27" s="79"/>
+      <c r="M27" s="79"/>
+      <c r="N27" s="80"/>
+      <c r="O27" s="100"/>
+      <c r="P27" s="90"/>
+      <c r="Q27" s="91"/>
       <c r="R27" s="1"/>
       <c r="AE27"/>
       <c r="AF27"/>
     </row>
     <row r="28" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="78"/>
-      <c r="C28" s="80"/>
-      <c r="D28" s="97"/>
-      <c r="E28" s="98"/>
-      <c r="F28" s="108"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="109"/>
-      <c r="I28" s="109"/>
-      <c r="J28" s="109"/>
-      <c r="K28" s="109"/>
-      <c r="L28" s="109"/>
-      <c r="M28" s="109"/>
-      <c r="N28" s="110"/>
-      <c r="O28" s="113"/>
-      <c r="P28" s="74"/>
-      <c r="Q28" s="75"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="81"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="83"/>
+      <c r="O28" s="100"/>
+      <c r="P28" s="90"/>
+      <c r="Q28" s="91"/>
       <c r="R28" s="1"/>
       <c r="AE28"/>
       <c r="AF28"/>
     </row>
     <row r="29" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="83">
+      <c r="B29" s="56">
         <v>4</v>
       </c>
-      <c r="C29" s="92"/>
-      <c r="D29" s="93"/>
-      <c r="E29" s="94"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="106"/>
-      <c r="H29" s="106"/>
-      <c r="I29" s="106"/>
-      <c r="J29" s="106"/>
-      <c r="K29" s="106"/>
-      <c r="L29" s="106"/>
-      <c r="M29" s="106"/>
-      <c r="N29" s="107"/>
-      <c r="O29" s="113"/>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="75"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="79"/>
+      <c r="L29" s="79"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="80"/>
+      <c r="O29" s="100"/>
+      <c r="P29" s="90"/>
+      <c r="Q29" s="91"/>
       <c r="R29" s="1"/>
       <c r="AE29"/>
       <c r="AF29"/>
     </row>
     <row r="30" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="77"/>
-      <c r="C30" s="79"/>
-      <c r="D30" s="95"/>
-      <c r="E30" s="96"/>
-      <c r="F30" s="105"/>
-      <c r="G30" s="106"/>
-      <c r="H30" s="106"/>
-      <c r="I30" s="106"/>
-      <c r="J30" s="106"/>
-      <c r="K30" s="106"/>
-      <c r="L30" s="106"/>
-      <c r="M30" s="106"/>
-      <c r="N30" s="107"/>
-      <c r="O30" s="113"/>
-      <c r="P30" s="74"/>
-      <c r="Q30" s="75"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79"/>
+      <c r="N30" s="80"/>
+      <c r="O30" s="100"/>
+      <c r="P30" s="90"/>
+      <c r="Q30" s="91"/>
       <c r="R30" s="1"/>
       <c r="AE30"/>
       <c r="AF30"/>
     </row>
     <row r="31" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="78"/>
-      <c r="C31" s="80"/>
-      <c r="D31" s="97"/>
-      <c r="E31" s="98"/>
-      <c r="F31" s="108"/>
-      <c r="G31" s="109"/>
-      <c r="H31" s="109"/>
-      <c r="I31" s="109"/>
-      <c r="J31" s="109"/>
-      <c r="K31" s="109"/>
-      <c r="L31" s="109"/>
-      <c r="M31" s="109"/>
-      <c r="N31" s="110"/>
-      <c r="O31" s="113"/>
-      <c r="P31" s="74"/>
-      <c r="Q31" s="75"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="95"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="82"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="82"/>
+      <c r="N31" s="83"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="90"/>
+      <c r="Q31" s="91"/>
       <c r="R31" s="1"/>
       <c r="AE31"/>
       <c r="AF31"/>
     </row>
     <row r="32" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="83">
+      <c r="B32" s="56">
         <v>5</v>
       </c>
-      <c r="C32" s="92"/>
-      <c r="D32" s="93"/>
-      <c r="E32" s="94"/>
-      <c r="F32" s="105"/>
-      <c r="G32" s="106"/>
-      <c r="H32" s="106"/>
-      <c r="I32" s="106"/>
-      <c r="J32" s="106"/>
-      <c r="K32" s="106"/>
-      <c r="L32" s="106"/>
-      <c r="M32" s="106"/>
-      <c r="N32" s="107"/>
-      <c r="O32" s="113"/>
-      <c r="P32" s="74"/>
-      <c r="Q32" s="75"/>
+      <c r="C32" s="96"/>
+      <c r="D32" s="67"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="79"/>
+      <c r="K32" s="79"/>
+      <c r="L32" s="79"/>
+      <c r="M32" s="79"/>
+      <c r="N32" s="80"/>
+      <c r="O32" s="100"/>
+      <c r="P32" s="90"/>
+      <c r="Q32" s="91"/>
       <c r="R32" s="1"/>
       <c r="AE32"/>
       <c r="AF32"/>
     </row>
     <row r="33" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="77"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="96"/>
-      <c r="F33" s="105"/>
-      <c r="G33" s="106"/>
-      <c r="H33" s="106"/>
-      <c r="I33" s="106"/>
-      <c r="J33" s="106"/>
-      <c r="K33" s="106"/>
-      <c r="L33" s="106"/>
-      <c r="M33" s="106"/>
-      <c r="N33" s="107"/>
-      <c r="O33" s="113"/>
-      <c r="P33" s="74"/>
-      <c r="Q33" s="75"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="79"/>
+      <c r="I33" s="79"/>
+      <c r="J33" s="79"/>
+      <c r="K33" s="79"/>
+      <c r="L33" s="79"/>
+      <c r="M33" s="79"/>
+      <c r="N33" s="80"/>
+      <c r="O33" s="100"/>
+      <c r="P33" s="90"/>
+      <c r="Q33" s="91"/>
       <c r="R33" s="1"/>
       <c r="AE33"/>
       <c r="AF33"/>
     </row>
     <row r="34" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="78"/>
-      <c r="C34" s="80"/>
-      <c r="D34" s="97"/>
-      <c r="E34" s="98"/>
-      <c r="F34" s="108"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="109"/>
-      <c r="I34" s="109"/>
-      <c r="J34" s="109"/>
-      <c r="K34" s="109"/>
-      <c r="L34" s="109"/>
-      <c r="M34" s="109"/>
-      <c r="N34" s="110"/>
-      <c r="O34" s="113"/>
-      <c r="P34" s="74"/>
-      <c r="Q34" s="75"/>
+      <c r="B34" s="55"/>
+      <c r="C34" s="95"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="81"/>
+      <c r="G34" s="82"/>
+      <c r="H34" s="82"/>
+      <c r="I34" s="82"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="82"/>
+      <c r="L34" s="82"/>
+      <c r="M34" s="82"/>
+      <c r="N34" s="83"/>
+      <c r="O34" s="100"/>
+      <c r="P34" s="90"/>
+      <c r="Q34" s="91"/>
       <c r="R34" s="1"/>
       <c r="AE34"/>
       <c r="AF34"/>
     </row>
     <row r="35" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="83">
+      <c r="B35" s="56">
         <v>6</v>
       </c>
-      <c r="C35" s="92"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="94"/>
-      <c r="F35" s="105"/>
-      <c r="G35" s="106"/>
-      <c r="H35" s="106"/>
-      <c r="I35" s="106"/>
-      <c r="J35" s="106"/>
-      <c r="K35" s="106"/>
-      <c r="L35" s="106"/>
-      <c r="M35" s="106"/>
-      <c r="N35" s="107"/>
-      <c r="O35" s="113"/>
-      <c r="P35" s="74"/>
-      <c r="Q35" s="75"/>
+      <c r="C35" s="96"/>
+      <c r="D35" s="67"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="80"/>
+      <c r="O35" s="100"/>
+      <c r="P35" s="90"/>
+      <c r="Q35" s="91"/>
       <c r="R35" s="1"/>
       <c r="AE35"/>
       <c r="AF35"/>
     </row>
     <row r="36" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="77"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="95"/>
-      <c r="E36" s="96"/>
-      <c r="F36" s="105"/>
-      <c r="G36" s="106"/>
-      <c r="H36" s="106"/>
-      <c r="I36" s="106"/>
-      <c r="J36" s="106"/>
-      <c r="K36" s="106"/>
-      <c r="L36" s="106"/>
-      <c r="M36" s="106"/>
-      <c r="N36" s="107"/>
-      <c r="O36" s="113"/>
-      <c r="P36" s="74"/>
-      <c r="Q36" s="75"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="78"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="79"/>
+      <c r="L36" s="79"/>
+      <c r="M36" s="79"/>
+      <c r="N36" s="80"/>
+      <c r="O36" s="100"/>
+      <c r="P36" s="90"/>
+      <c r="Q36" s="91"/>
       <c r="R36" s="1"/>
       <c r="AE36"/>
       <c r="AF36"/>
     </row>
     <row r="37" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="78"/>
-      <c r="C37" s="80"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="98"/>
-      <c r="F37" s="108"/>
-      <c r="G37" s="109"/>
-      <c r="H37" s="109"/>
-      <c r="I37" s="109"/>
-      <c r="J37" s="109"/>
-      <c r="K37" s="109"/>
-      <c r="L37" s="109"/>
-      <c r="M37" s="109"/>
-      <c r="N37" s="110"/>
-      <c r="O37" s="113"/>
-      <c r="P37" s="74"/>
-      <c r="Q37" s="75"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="95"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="81"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="82"/>
+      <c r="N37" s="83"/>
+      <c r="O37" s="100"/>
+      <c r="P37" s="90"/>
+      <c r="Q37" s="91"/>
       <c r="R37" s="1"/>
       <c r="AE37"/>
       <c r="AF37"/>
     </row>
     <row r="38" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="83">
+      <c r="B38" s="56">
         <v>7</v>
       </c>
-      <c r="C38" s="92"/>
-      <c r="D38" s="93"/>
-      <c r="E38" s="94"/>
-      <c r="F38" s="105"/>
-      <c r="G38" s="106"/>
-      <c r="H38" s="106"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="106"/>
-      <c r="K38" s="106"/>
-      <c r="L38" s="106"/>
-      <c r="M38" s="106"/>
-      <c r="N38" s="107"/>
-      <c r="O38" s="113"/>
-      <c r="P38" s="74"/>
-      <c r="Q38" s="75"/>
+      <c r="C38" s="96"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="79"/>
+      <c r="H38" s="79"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="79"/>
+      <c r="M38" s="79"/>
+      <c r="N38" s="80"/>
+      <c r="O38" s="100"/>
+      <c r="P38" s="90"/>
+      <c r="Q38" s="91"/>
       <c r="R38" s="1"/>
       <c r="AE38"/>
       <c r="AF38"/>
     </row>
     <row r="39" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="77"/>
-      <c r="C39" s="79"/>
-      <c r="D39" s="95"/>
-      <c r="E39" s="96"/>
-      <c r="F39" s="105"/>
-      <c r="G39" s="106"/>
-      <c r="H39" s="106"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="106"/>
-      <c r="K39" s="106"/>
-      <c r="L39" s="106"/>
-      <c r="M39" s="106"/>
-      <c r="N39" s="107"/>
-      <c r="O39" s="113"/>
-      <c r="P39" s="74"/>
-      <c r="Q39" s="75"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="94"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="78"/>
+      <c r="G39" s="79"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="79"/>
+      <c r="J39" s="79"/>
+      <c r="K39" s="79"/>
+      <c r="L39" s="79"/>
+      <c r="M39" s="79"/>
+      <c r="N39" s="80"/>
+      <c r="O39" s="100"/>
+      <c r="P39" s="90"/>
+      <c r="Q39" s="91"/>
       <c r="R39" s="1"/>
       <c r="AE39"/>
       <c r="AF39"/>
     </row>
     <row r="40" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="78"/>
-      <c r="C40" s="80"/>
-      <c r="D40" s="97"/>
-      <c r="E40" s="98"/>
-      <c r="F40" s="108"/>
-      <c r="G40" s="109"/>
-      <c r="H40" s="109"/>
-      <c r="I40" s="109"/>
-      <c r="J40" s="109"/>
-      <c r="K40" s="109"/>
-      <c r="L40" s="109"/>
-      <c r="M40" s="109"/>
-      <c r="N40" s="110"/>
-      <c r="O40" s="113"/>
-      <c r="P40" s="74"/>
-      <c r="Q40" s="75"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="95"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="81"/>
+      <c r="G40" s="82"/>
+      <c r="H40" s="82"/>
+      <c r="I40" s="82"/>
+      <c r="J40" s="82"/>
+      <c r="K40" s="82"/>
+      <c r="L40" s="82"/>
+      <c r="M40" s="82"/>
+      <c r="N40" s="83"/>
+      <c r="O40" s="100"/>
+      <c r="P40" s="90"/>
+      <c r="Q40" s="91"/>
       <c r="R40" s="1"/>
       <c r="AE40"/>
       <c r="AF40"/>
     </row>
     <row r="41" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="83">
+      <c r="B41" s="56">
         <v>8</v>
       </c>
-      <c r="C41" s="92"/>
-      <c r="D41" s="93"/>
-      <c r="E41" s="94"/>
-      <c r="F41" s="105"/>
-      <c r="G41" s="106"/>
-      <c r="H41" s="106"/>
-      <c r="I41" s="106"/>
-      <c r="J41" s="106"/>
-      <c r="K41" s="106"/>
-      <c r="L41" s="106"/>
-      <c r="M41" s="106"/>
-      <c r="N41" s="107"/>
-      <c r="O41" s="103"/>
-      <c r="P41" s="74"/>
-      <c r="Q41" s="75"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="79"/>
+      <c r="H41" s="79"/>
+      <c r="I41" s="79"/>
+      <c r="J41" s="79"/>
+      <c r="K41" s="79"/>
+      <c r="L41" s="79"/>
+      <c r="M41" s="79"/>
+      <c r="N41" s="80"/>
+      <c r="O41" s="106"/>
+      <c r="P41" s="90"/>
+      <c r="Q41" s="91"/>
       <c r="R41" s="1"/>
       <c r="AE41"/>
       <c r="AF41"/>
     </row>
     <row r="42" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="77"/>
-      <c r="C42" s="79"/>
-      <c r="D42" s="95"/>
-      <c r="E42" s="96"/>
-      <c r="F42" s="105"/>
-      <c r="G42" s="106"/>
-      <c r="H42" s="106"/>
-      <c r="I42" s="106"/>
-      <c r="J42" s="106"/>
-      <c r="K42" s="106"/>
-      <c r="L42" s="106"/>
-      <c r="M42" s="106"/>
-      <c r="N42" s="107"/>
-      <c r="O42" s="103"/>
-      <c r="P42" s="74"/>
-      <c r="Q42" s="75"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="94"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="78"/>
+      <c r="G42" s="79"/>
+      <c r="H42" s="79"/>
+      <c r="I42" s="79"/>
+      <c r="J42" s="79"/>
+      <c r="K42" s="79"/>
+      <c r="L42" s="79"/>
+      <c r="M42" s="79"/>
+      <c r="N42" s="80"/>
+      <c r="O42" s="106"/>
+      <c r="P42" s="90"/>
+      <c r="Q42" s="91"/>
       <c r="R42" s="1"/>
       <c r="AE42"/>
       <c r="AF42"/>
     </row>
     <row r="43" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="78"/>
-      <c r="C43" s="80"/>
-      <c r="D43" s="97"/>
-      <c r="E43" s="98"/>
-      <c r="F43" s="108"/>
-      <c r="G43" s="109"/>
-      <c r="H43" s="109"/>
-      <c r="I43" s="109"/>
-      <c r="J43" s="109"/>
-      <c r="K43" s="109"/>
-      <c r="L43" s="109"/>
-      <c r="M43" s="109"/>
-      <c r="N43" s="110"/>
-      <c r="O43" s="104"/>
-      <c r="P43" s="74"/>
-      <c r="Q43" s="75"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="81"/>
+      <c r="G43" s="82"/>
+      <c r="H43" s="82"/>
+      <c r="I43" s="82"/>
+      <c r="J43" s="82"/>
+      <c r="K43" s="82"/>
+      <c r="L43" s="82"/>
+      <c r="M43" s="82"/>
+      <c r="N43" s="83"/>
+      <c r="O43" s="107"/>
+      <c r="P43" s="90"/>
+      <c r="Q43" s="91"/>
       <c r="R43" s="1"/>
       <c r="AE43"/>
       <c r="AF43"/>
@@ -3166,20 +3177,20 @@
         <v>31</v>
       </c>
       <c r="C45"/>
-      <c r="D45" s="76"/>
-      <c r="E45" s="76"/>
-      <c r="F45" s="76"/>
-      <c r="G45" s="76"/>
-      <c r="H45" s="76"/>
-      <c r="I45" s="76"/>
-      <c r="J45" s="76"/>
-      <c r="K45" s="76"/>
-      <c r="L45" s="76"/>
-      <c r="M45" s="76"/>
-      <c r="N45" s="76"/>
-      <c r="O45" s="76"/>
-      <c r="P45" s="76"/>
-      <c r="Q45" s="76"/>
+      <c r="D45" s="108"/>
+      <c r="E45" s="108"/>
+      <c r="F45" s="108"/>
+      <c r="G45" s="108"/>
+      <c r="H45" s="108"/>
+      <c r="I45" s="108"/>
+      <c r="J45" s="108"/>
+      <c r="K45" s="108"/>
+      <c r="L45" s="108"/>
+      <c r="M45" s="108"/>
+      <c r="N45" s="108"/>
+      <c r="O45" s="108"/>
+      <c r="P45" s="108"/>
+      <c r="Q45" s="108"/>
       <c r="R45" s="6"/>
       <c r="AE45"/>
       <c r="AF45"/>
@@ -3188,20 +3199,20 @@
       <c r="A46" s="1"/>
       <c r="B46" s="6"/>
       <c r="C46"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="73"/>
-      <c r="J46" s="73"/>
-      <c r="K46" s="73"/>
-      <c r="L46" s="73"/>
-      <c r="M46" s="73"/>
-      <c r="N46" s="73"/>
-      <c r="O46" s="73"/>
-      <c r="P46" s="73"/>
-      <c r="Q46" s="73"/>
+      <c r="D46" s="109"/>
+      <c r="E46" s="109"/>
+      <c r="F46" s="109"/>
+      <c r="G46" s="109"/>
+      <c r="H46" s="109"/>
+      <c r="I46" s="109"/>
+      <c r="J46" s="109"/>
+      <c r="K46" s="109"/>
+      <c r="L46" s="109"/>
+      <c r="M46" s="109"/>
+      <c r="N46" s="109"/>
+      <c r="O46" s="109"/>
+      <c r="P46" s="109"/>
+      <c r="Q46" s="109"/>
       <c r="R46" s="6"/>
       <c r="AE46"/>
       <c r="AF46"/>
@@ -3210,20 +3221,20 @@
       <c r="A47" s="1"/>
       <c r="B47" s="6"/>
       <c r="C47"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="73"/>
-      <c r="F47" s="73"/>
-      <c r="G47" s="73"/>
-      <c r="H47" s="73"/>
-      <c r="I47" s="73"/>
-      <c r="J47" s="73"/>
-      <c r="K47" s="73"/>
-      <c r="L47" s="73"/>
-      <c r="M47" s="73"/>
-      <c r="N47" s="73"/>
-      <c r="O47" s="73"/>
-      <c r="P47" s="73"/>
-      <c r="Q47" s="73"/>
+      <c r="D47" s="109"/>
+      <c r="E47" s="109"/>
+      <c r="F47" s="109"/>
+      <c r="G47" s="109"/>
+      <c r="H47" s="109"/>
+      <c r="I47" s="109"/>
+      <c r="J47" s="109"/>
+      <c r="K47" s="109"/>
+      <c r="L47" s="109"/>
+      <c r="M47" s="109"/>
+      <c r="N47" s="109"/>
+      <c r="O47" s="109"/>
+      <c r="P47" s="109"/>
+      <c r="Q47" s="109"/>
       <c r="R47" s="6"/>
       <c r="AE47"/>
       <c r="AF47"/>
@@ -3298,26 +3309,26 @@
     </row>
     <row r="51" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="81" t="s">
+      <c r="B51" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="81" t="s">
+      <c r="C51" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="99" t="s">
+      <c r="D51" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="100"/>
-      <c r="F51" s="100"/>
-      <c r="G51" s="100"/>
-      <c r="H51" s="100"/>
-      <c r="I51" s="100"/>
-      <c r="J51" s="100"/>
-      <c r="K51" s="100"/>
-      <c r="L51" s="100"/>
-      <c r="M51" s="100"/>
-      <c r="N51" s="100"/>
-      <c r="O51" s="100"/>
+      <c r="E51" s="70"/>
+      <c r="F51" s="70"/>
+      <c r="G51" s="70"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="70"/>
+      <c r="J51" s="70"/>
+      <c r="K51" s="70"/>
+      <c r="L51" s="70"/>
+      <c r="M51" s="70"/>
+      <c r="N51" s="70"/>
+      <c r="O51" s="70"/>
       <c r="P51" s="84" t="s">
         <v>47</v>
       </c>
@@ -3328,20 +3339,20 @@
     </row>
     <row r="52" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="82"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="101"/>
-      <c r="E52" s="102"/>
-      <c r="F52" s="102"/>
-      <c r="G52" s="102"/>
-      <c r="H52" s="102"/>
-      <c r="I52" s="102"/>
-      <c r="J52" s="102"/>
-      <c r="K52" s="102"/>
-      <c r="L52" s="102"/>
-      <c r="M52" s="102"/>
-      <c r="N52" s="102"/>
-      <c r="O52" s="102"/>
+      <c r="B52" s="98"/>
+      <c r="C52" s="98"/>
+      <c r="D52" s="72"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="73"/>
+      <c r="G52" s="73"/>
+      <c r="H52" s="73"/>
+      <c r="I52" s="73"/>
+      <c r="J52" s="73"/>
+      <c r="K52" s="73"/>
+      <c r="L52" s="73"/>
+      <c r="M52" s="73"/>
+      <c r="N52" s="73"/>
+      <c r="O52" s="73"/>
       <c r="P52" s="86"/>
       <c r="Q52" s="87"/>
       <c r="R52" s="1"/>
@@ -3350,10 +3361,10 @@
     </row>
     <row r="53" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
-      <c r="B53" s="77" t="s">
+      <c r="B53" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="79"/>
+      <c r="C53" s="94"/>
       <c r="D53" s="21"/>
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
@@ -3366,14 +3377,14 @@
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
       <c r="O53" s="22"/>
-      <c r="P53" s="88"/>
-      <c r="Q53" s="89"/>
+      <c r="P53" s="110"/>
+      <c r="Q53" s="111"/>
       <c r="R53" s="1"/>
     </row>
     <row r="54" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
-      <c r="B54" s="77"/>
-      <c r="C54" s="79"/>
+      <c r="B54" s="54"/>
+      <c r="C54" s="94"/>
       <c r="D54" s="24"/>
       <c r="E54" s="25"/>
       <c r="F54" s="25"/>
@@ -3386,14 +3397,14 @@
       <c r="M54" s="25"/>
       <c r="N54" s="25"/>
       <c r="O54" s="25"/>
-      <c r="P54" s="90"/>
-      <c r="Q54" s="91"/>
+      <c r="P54" s="112"/>
+      <c r="Q54" s="113"/>
       <c r="R54" s="1"/>
     </row>
     <row r="55" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
-      <c r="B55" s="78"/>
-      <c r="C55" s="80"/>
+      <c r="B55" s="55"/>
+      <c r="C55" s="95"/>
       <c r="D55" s="23"/>
       <c r="E55" s="20"/>
       <c r="F55" s="20"/>
@@ -3406,16 +3417,16 @@
       <c r="M55" s="20"/>
       <c r="N55" s="20"/>
       <c r="O55" s="20"/>
-      <c r="P55" s="90"/>
-      <c r="Q55" s="91"/>
+      <c r="P55" s="112"/>
+      <c r="Q55" s="113"/>
       <c r="R55" s="1"/>
     </row>
     <row r="56" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
-      <c r="B56" s="83" t="s">
+      <c r="B56" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="92"/>
+      <c r="C56" s="96"/>
       <c r="D56" s="24"/>
       <c r="E56" s="25"/>
       <c r="F56" s="25"/>
@@ -3428,14 +3439,14 @@
       <c r="M56" s="25"/>
       <c r="N56" s="25"/>
       <c r="O56" s="25"/>
-      <c r="P56" s="90"/>
-      <c r="Q56" s="91"/>
+      <c r="P56" s="112"/>
+      <c r="Q56" s="113"/>
       <c r="R56" s="1"/>
     </row>
     <row r="57" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
-      <c r="B57" s="77"/>
-      <c r="C57" s="79"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="94"/>
       <c r="D57" s="24"/>
       <c r="E57" s="25"/>
       <c r="F57" s="25"/>
@@ -3448,14 +3459,14 @@
       <c r="M57" s="25"/>
       <c r="N57" s="25"/>
       <c r="O57" s="25"/>
-      <c r="P57" s="90"/>
-      <c r="Q57" s="91"/>
+      <c r="P57" s="112"/>
+      <c r="Q57" s="113"/>
       <c r="R57" s="1"/>
     </row>
     <row r="58" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
-      <c r="B58" s="78"/>
-      <c r="C58" s="80"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="95"/>
       <c r="D58" s="23"/>
       <c r="E58" s="20"/>
       <c r="F58" s="20"/>
@@ -3468,8 +3479,8 @@
       <c r="M58" s="20"/>
       <c r="N58" s="20"/>
       <c r="O58" s="20"/>
-      <c r="P58" s="90"/>
-      <c r="Q58" s="91"/>
+      <c r="P58" s="112"/>
+      <c r="Q58" s="113"/>
       <c r="R58" s="1"/>
     </row>
     <row r="59" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3498,20 +3509,20 @@
         <v>30</v>
       </c>
       <c r="C60"/>
-      <c r="D60" s="76"/>
-      <c r="E60" s="76"/>
-      <c r="F60" s="76"/>
-      <c r="G60" s="76"/>
-      <c r="H60" s="76"/>
-      <c r="I60" s="76"/>
-      <c r="J60" s="76"/>
-      <c r="K60" s="76"/>
-      <c r="L60" s="76"/>
-      <c r="M60" s="76"/>
-      <c r="N60" s="76"/>
-      <c r="O60" s="76"/>
-      <c r="P60" s="76"/>
-      <c r="Q60" s="76"/>
+      <c r="D60" s="108"/>
+      <c r="E60" s="108"/>
+      <c r="F60" s="108"/>
+      <c r="G60" s="108"/>
+      <c r="H60" s="108"/>
+      <c r="I60" s="108"/>
+      <c r="J60" s="108"/>
+      <c r="K60" s="108"/>
+      <c r="L60" s="108"/>
+      <c r="M60" s="108"/>
+      <c r="N60" s="108"/>
+      <c r="O60" s="108"/>
+      <c r="P60" s="108"/>
+      <c r="Q60" s="108"/>
       <c r="R60" s="6"/>
     </row>
     <row r="61" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3538,20 +3549,20 @@
       <c r="A62" s="1"/>
       <c r="B62" s="6"/>
       <c r="C62"/>
-      <c r="D62" s="73"/>
-      <c r="E62" s="73"/>
-      <c r="F62" s="73"/>
-      <c r="G62" s="73"/>
-      <c r="H62" s="73"/>
-      <c r="I62" s="73"/>
-      <c r="J62" s="73"/>
-      <c r="K62" s="73"/>
-      <c r="L62" s="73"/>
-      <c r="M62" s="73"/>
-      <c r="N62" s="73"/>
-      <c r="O62" s="73"/>
-      <c r="P62" s="73"/>
-      <c r="Q62" s="73"/>
+      <c r="D62" s="109"/>
+      <c r="E62" s="109"/>
+      <c r="F62" s="109"/>
+      <c r="G62" s="109"/>
+      <c r="H62" s="109"/>
+      <c r="I62" s="109"/>
+      <c r="J62" s="109"/>
+      <c r="K62" s="109"/>
+      <c r="L62" s="109"/>
+      <c r="M62" s="109"/>
+      <c r="N62" s="109"/>
+      <c r="O62" s="109"/>
+      <c r="P62" s="109"/>
+      <c r="Q62" s="109"/>
       <c r="R62" s="6"/>
     </row>
     <row r="63" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3697,21 +3708,21 @@
       <c r="B68" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="111"/>
-      <c r="D68" s="111"/>
-      <c r="E68" s="111"/>
-      <c r="F68" s="111"/>
-      <c r="G68" s="111"/>
-      <c r="H68" s="111"/>
-      <c r="I68" s="111"/>
-      <c r="J68" s="111"/>
-      <c r="K68" s="111"/>
-      <c r="L68" s="111"/>
-      <c r="M68" s="111"/>
-      <c r="N68" s="111"/>
-      <c r="O68" s="111"/>
-      <c r="P68" s="111"/>
-      <c r="Q68" s="111"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
+      <c r="G68" s="50"/>
+      <c r="H68" s="50"/>
+      <c r="I68" s="50"/>
+      <c r="J68" s="50"/>
+      <c r="K68" s="50"/>
+      <c r="L68" s="50"/>
+      <c r="M68" s="50"/>
+      <c r="N68" s="50"/>
+      <c r="O68" s="50"/>
+      <c r="P68" s="50"/>
+      <c r="Q68" s="50"/>
       <c r="R68" s="6"/>
       <c r="S68" s="14"/>
       <c r="T68" s="14"/>
@@ -3725,21 +3736,21 @@
     <row r="69" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="C69" s="112"/>
-      <c r="D69" s="112"/>
-      <c r="E69" s="112"/>
-      <c r="F69" s="112"/>
-      <c r="G69" s="112"/>
-      <c r="H69" s="112"/>
-      <c r="I69" s="112"/>
-      <c r="J69" s="112"/>
-      <c r="K69" s="112"/>
-      <c r="L69" s="112"/>
-      <c r="M69" s="112"/>
-      <c r="N69" s="112"/>
-      <c r="O69" s="112"/>
-      <c r="P69" s="112"/>
-      <c r="Q69" s="112"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="51"/>
+      <c r="E69" s="51"/>
+      <c r="F69" s="51"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="51"/>
+      <c r="I69" s="51"/>
+      <c r="J69" s="51"/>
+      <c r="K69" s="51"/>
+      <c r="L69" s="51"/>
+      <c r="M69" s="51"/>
+      <c r="N69" s="51"/>
+      <c r="O69" s="51"/>
+      <c r="P69" s="51"/>
+      <c r="Q69" s="51"/>
       <c r="R69" s="6"/>
       <c r="S69" s="14"/>
       <c r="T69" s="14"/>
@@ -3843,21 +3854,21 @@
       <c r="B73" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C73" s="111"/>
-      <c r="D73" s="111"/>
-      <c r="E73" s="111"/>
-      <c r="F73" s="111"/>
-      <c r="G73" s="111"/>
-      <c r="H73" s="111"/>
-      <c r="I73" s="111"/>
-      <c r="J73" s="111"/>
-      <c r="K73" s="111"/>
-      <c r="L73" s="111"/>
-      <c r="M73" s="111"/>
-      <c r="N73" s="111"/>
-      <c r="O73" s="111"/>
-      <c r="P73" s="111"/>
-      <c r="Q73" s="111"/>
+      <c r="C73" s="50"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="50"/>
+      <c r="F73" s="50"/>
+      <c r="G73" s="50"/>
+      <c r="H73" s="50"/>
+      <c r="I73" s="50"/>
+      <c r="J73" s="50"/>
+      <c r="K73" s="50"/>
+      <c r="L73" s="50"/>
+      <c r="M73" s="50"/>
+      <c r="N73" s="50"/>
+      <c r="O73" s="50"/>
+      <c r="P73" s="50"/>
+      <c r="Q73" s="50"/>
       <c r="R73" s="6"/>
       <c r="S73" s="14"/>
       <c r="T73" s="14"/>
@@ -3871,21 +3882,21 @@
     <row r="74" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-      <c r="C74" s="112"/>
-      <c r="D74" s="112"/>
-      <c r="E74" s="112"/>
-      <c r="F74" s="112"/>
-      <c r="G74" s="112"/>
-      <c r="H74" s="112"/>
-      <c r="I74" s="112"/>
-      <c r="J74" s="112"/>
-      <c r="K74" s="112"/>
-      <c r="L74" s="112"/>
-      <c r="M74" s="112"/>
-      <c r="N74" s="112"/>
-      <c r="O74" s="112"/>
-      <c r="P74" s="112"/>
-      <c r="Q74" s="112"/>
+      <c r="C74" s="51"/>
+      <c r="D74" s="51"/>
+      <c r="E74" s="51"/>
+      <c r="F74" s="51"/>
+      <c r="G74" s="51"/>
+      <c r="H74" s="51"/>
+      <c r="I74" s="51"/>
+      <c r="J74" s="51"/>
+      <c r="K74" s="51"/>
+      <c r="L74" s="51"/>
+      <c r="M74" s="51"/>
+      <c r="N74" s="51"/>
+      <c r="O74" s="51"/>
+      <c r="P74" s="51"/>
+      <c r="Q74" s="51"/>
       <c r="R74" s="6"/>
       <c r="S74" s="14"/>
       <c r="T74" s="14"/>
@@ -3989,21 +4000,21 @@
       <c r="B78" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C78" s="111"/>
-      <c r="D78" s="111"/>
-      <c r="E78" s="111"/>
-      <c r="F78" s="111"/>
-      <c r="G78" s="111"/>
-      <c r="H78" s="111"/>
-      <c r="I78" s="111"/>
-      <c r="J78" s="111"/>
-      <c r="K78" s="111"/>
-      <c r="L78" s="111"/>
-      <c r="M78" s="111"/>
-      <c r="N78" s="111"/>
-      <c r="O78" s="111"/>
-      <c r="P78" s="111"/>
-      <c r="Q78" s="111"/>
+      <c r="C78" s="50"/>
+      <c r="D78" s="50"/>
+      <c r="E78" s="50"/>
+      <c r="F78" s="50"/>
+      <c r="G78" s="50"/>
+      <c r="H78" s="50"/>
+      <c r="I78" s="50"/>
+      <c r="J78" s="50"/>
+      <c r="K78" s="50"/>
+      <c r="L78" s="50"/>
+      <c r="M78" s="50"/>
+      <c r="N78" s="50"/>
+      <c r="O78" s="50"/>
+      <c r="P78" s="50"/>
+      <c r="Q78" s="50"/>
       <c r="R78" s="6"/>
       <c r="S78" s="14"/>
       <c r="T78" s="14"/>
@@ -4017,21 +4028,21 @@
     <row r="79" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="C79" s="112"/>
-      <c r="D79" s="112"/>
-      <c r="E79" s="112"/>
-      <c r="F79" s="112"/>
-      <c r="G79" s="112"/>
-      <c r="H79" s="112"/>
-      <c r="I79" s="112"/>
-      <c r="J79" s="112"/>
-      <c r="K79" s="112"/>
-      <c r="L79" s="112"/>
-      <c r="M79" s="112"/>
-      <c r="N79" s="112"/>
-      <c r="O79" s="112"/>
-      <c r="P79" s="112"/>
-      <c r="Q79" s="112"/>
+      <c r="C79" s="51"/>
+      <c r="D79" s="51"/>
+      <c r="E79" s="51"/>
+      <c r="F79" s="51"/>
+      <c r="G79" s="51"/>
+      <c r="H79" s="51"/>
+      <c r="I79" s="51"/>
+      <c r="J79" s="51"/>
+      <c r="K79" s="51"/>
+      <c r="L79" s="51"/>
+      <c r="M79" s="51"/>
+      <c r="N79" s="51"/>
+      <c r="O79" s="51"/>
+      <c r="P79" s="51"/>
+      <c r="Q79" s="51"/>
       <c r="R79" s="6"/>
       <c r="S79" s="14"/>
       <c r="T79" s="14"/>
@@ -4135,21 +4146,21 @@
       <c r="B83" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C83" s="111"/>
-      <c r="D83" s="111"/>
-      <c r="E83" s="111"/>
-      <c r="F83" s="111"/>
-      <c r="G83" s="111"/>
-      <c r="H83" s="111"/>
-      <c r="I83" s="111"/>
-      <c r="J83" s="111"/>
-      <c r="K83" s="111"/>
-      <c r="L83" s="111"/>
-      <c r="M83" s="111"/>
-      <c r="N83" s="111"/>
-      <c r="O83" s="111"/>
-      <c r="P83" s="111"/>
-      <c r="Q83" s="111"/>
+      <c r="C83" s="50"/>
+      <c r="D83" s="50"/>
+      <c r="E83" s="50"/>
+      <c r="F83" s="50"/>
+      <c r="G83" s="50"/>
+      <c r="H83" s="50"/>
+      <c r="I83" s="50"/>
+      <c r="J83" s="50"/>
+      <c r="K83" s="50"/>
+      <c r="L83" s="50"/>
+      <c r="M83" s="50"/>
+      <c r="N83" s="50"/>
+      <c r="O83" s="50"/>
+      <c r="P83" s="50"/>
+      <c r="Q83" s="50"/>
       <c r="R83" s="6"/>
       <c r="S83" s="14"/>
       <c r="T83" s="14"/>
@@ -4163,21 +4174,21 @@
     <row r="84" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
-      <c r="C84" s="112"/>
-      <c r="D84" s="112"/>
-      <c r="E84" s="112"/>
-      <c r="F84" s="112"/>
-      <c r="G84" s="112"/>
-      <c r="H84" s="112"/>
-      <c r="I84" s="112"/>
-      <c r="J84" s="112"/>
-      <c r="K84" s="112"/>
-      <c r="L84" s="112"/>
-      <c r="M84" s="112"/>
-      <c r="N84" s="112"/>
-      <c r="O84" s="112"/>
-      <c r="P84" s="112"/>
-      <c r="Q84" s="112"/>
+      <c r="C84" s="51"/>
+      <c r="D84" s="51"/>
+      <c r="E84" s="51"/>
+      <c r="F84" s="51"/>
+      <c r="G84" s="51"/>
+      <c r="H84" s="51"/>
+      <c r="I84" s="51"/>
+      <c r="J84" s="51"/>
+      <c r="K84" s="51"/>
+      <c r="L84" s="51"/>
+      <c r="M84" s="51"/>
+      <c r="N84" s="51"/>
+      <c r="O84" s="51"/>
+      <c r="P84" s="51"/>
+      <c r="Q84" s="51"/>
       <c r="R84" s="6"/>
       <c r="S84" s="14"/>
       <c r="T84" s="14"/>
@@ -4281,21 +4292,21 @@
       <c r="B88" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C88" s="111"/>
-      <c r="D88" s="111"/>
-      <c r="E88" s="111"/>
-      <c r="F88" s="111"/>
-      <c r="G88" s="111"/>
-      <c r="H88" s="111"/>
-      <c r="I88" s="111"/>
-      <c r="J88" s="111"/>
-      <c r="K88" s="111"/>
-      <c r="L88" s="111"/>
-      <c r="M88" s="111"/>
-      <c r="N88" s="111"/>
-      <c r="O88" s="111"/>
-      <c r="P88" s="111"/>
-      <c r="Q88" s="111"/>
+      <c r="C88" s="50"/>
+      <c r="D88" s="50"/>
+      <c r="E88" s="50"/>
+      <c r="F88" s="50"/>
+      <c r="G88" s="50"/>
+      <c r="H88" s="50"/>
+      <c r="I88" s="50"/>
+      <c r="J88" s="50"/>
+      <c r="K88" s="50"/>
+      <c r="L88" s="50"/>
+      <c r="M88" s="50"/>
+      <c r="N88" s="50"/>
+      <c r="O88" s="50"/>
+      <c r="P88" s="50"/>
+      <c r="Q88" s="50"/>
       <c r="R88" s="6"/>
       <c r="S88" s="14"/>
       <c r="T88" s="14"/>
@@ -4309,21 +4320,21 @@
     <row r="89" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
-      <c r="C89" s="112"/>
-      <c r="D89" s="112"/>
-      <c r="E89" s="112"/>
-      <c r="F89" s="112"/>
-      <c r="G89" s="112"/>
-      <c r="H89" s="112"/>
-      <c r="I89" s="112"/>
-      <c r="J89" s="112"/>
-      <c r="K89" s="112"/>
-      <c r="L89" s="112"/>
-      <c r="M89" s="112"/>
-      <c r="N89" s="112"/>
-      <c r="O89" s="112"/>
-      <c r="P89" s="112"/>
-      <c r="Q89" s="112"/>
+      <c r="C89" s="51"/>
+      <c r="D89" s="51"/>
+      <c r="E89" s="51"/>
+      <c r="F89" s="51"/>
+      <c r="G89" s="51"/>
+      <c r="H89" s="51"/>
+      <c r="I89" s="51"/>
+      <c r="J89" s="51"/>
+      <c r="K89" s="51"/>
+      <c r="L89" s="51"/>
+      <c r="M89" s="51"/>
+      <c r="N89" s="51"/>
+      <c r="O89" s="51"/>
+      <c r="P89" s="51"/>
+      <c r="Q89" s="51"/>
       <c r="R89" s="6"/>
       <c r="S89" s="14"/>
       <c r="T89" s="14"/>
@@ -4391,10 +4402,10 @@
       <c r="U91" s="14"/>
       <c r="V91" s="14"/>
       <c r="W91" s="1"/>
-      <c r="X91" s="52"/>
-      <c r="Y91" s="52"/>
-      <c r="Z91" s="52"/>
-      <c r="AA91" s="52"/>
+      <c r="X91" s="105"/>
+      <c r="Y91" s="105"/>
+      <c r="Z91" s="105"/>
+      <c r="AA91" s="105"/>
     </row>
     <row r="92" spans="1:27" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
@@ -4420,41 +4431,41 @@
       <c r="U92" s="14"/>
       <c r="V92" s="14"/>
       <c r="W92" s="1"/>
-      <c r="X92" s="52"/>
-      <c r="Y92" s="52"/>
-      <c r="Z92" s="52"/>
-      <c r="AA92" s="52"/>
+      <c r="X92" s="105"/>
+      <c r="Y92" s="105"/>
+      <c r="Z92" s="105"/>
+      <c r="AA92" s="105"/>
     </row>
     <row r="93" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C93" s="111"/>
-      <c r="D93" s="111"/>
-      <c r="E93" s="111"/>
-      <c r="F93" s="111"/>
-      <c r="G93" s="111"/>
-      <c r="H93" s="111"/>
-      <c r="I93" s="111"/>
-      <c r="J93" s="111"/>
-      <c r="K93" s="111"/>
-      <c r="L93" s="111"/>
-      <c r="M93" s="111"/>
-      <c r="N93" s="111"/>
-      <c r="O93" s="111"/>
-      <c r="P93" s="111"/>
-      <c r="Q93" s="111"/>
+      <c r="C93" s="50"/>
+      <c r="D93" s="50"/>
+      <c r="E93" s="50"/>
+      <c r="F93" s="50"/>
+      <c r="G93" s="50"/>
+      <c r="H93" s="50"/>
+      <c r="I93" s="50"/>
+      <c r="J93" s="50"/>
+      <c r="K93" s="50"/>
+      <c r="L93" s="50"/>
+      <c r="M93" s="50"/>
+      <c r="N93" s="50"/>
+      <c r="O93" s="50"/>
+      <c r="P93" s="50"/>
+      <c r="Q93" s="50"/>
       <c r="R93" s="6"/>
       <c r="S93" s="14"/>
       <c r="T93" s="14"/>
       <c r="U93" s="14"/>
       <c r="V93" s="14"/>
       <c r="W93" s="1"/>
-      <c r="X93" s="52"/>
-      <c r="Y93" s="52"/>
-      <c r="Z93" s="52"/>
-      <c r="AA93" s="52"/>
+      <c r="X93" s="105"/>
+      <c r="Y93" s="105"/>
+      <c r="Z93" s="105"/>
+      <c r="AA93" s="105"/>
     </row>
     <row r="94" spans="1:27" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
@@ -4572,21 +4583,21 @@
       <c r="B98" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C98" s="111"/>
-      <c r="D98" s="111"/>
-      <c r="E98" s="111"/>
-      <c r="F98" s="111"/>
-      <c r="G98" s="111"/>
-      <c r="H98" s="111"/>
-      <c r="I98" s="111"/>
-      <c r="J98" s="111"/>
-      <c r="K98" s="111"/>
-      <c r="L98" s="111"/>
-      <c r="M98" s="111"/>
-      <c r="N98" s="111"/>
-      <c r="O98" s="111"/>
-      <c r="P98" s="111"/>
-      <c r="Q98" s="111"/>
+      <c r="C98" s="50"/>
+      <c r="D98" s="50"/>
+      <c r="E98" s="50"/>
+      <c r="F98" s="50"/>
+      <c r="G98" s="50"/>
+      <c r="H98" s="50"/>
+      <c r="I98" s="50"/>
+      <c r="J98" s="50"/>
+      <c r="K98" s="50"/>
+      <c r="L98" s="50"/>
+      <c r="M98" s="50"/>
+      <c r="N98" s="50"/>
+      <c r="O98" s="50"/>
+      <c r="P98" s="50"/>
+      <c r="Q98" s="50"/>
       <c r="R98" s="6"/>
       <c r="S98" s="14"/>
       <c r="T98" s="14"/>
@@ -4703,21 +4714,21 @@
       <c r="B103" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C103" s="131"/>
-      <c r="D103" s="131"/>
-      <c r="E103" s="131"/>
-      <c r="F103" s="131"/>
-      <c r="G103" s="131"/>
-      <c r="H103" s="131"/>
-      <c r="I103" s="131"/>
-      <c r="J103" s="131"/>
-      <c r="K103" s="131"/>
-      <c r="L103" s="131"/>
-      <c r="M103" s="131"/>
-      <c r="N103" s="131"/>
-      <c r="O103" s="131"/>
-      <c r="P103" s="131"/>
-      <c r="Q103" s="131"/>
+      <c r="C103" s="49"/>
+      <c r="D103" s="49"/>
+      <c r="E103" s="49"/>
+      <c r="F103" s="49"/>
+      <c r="G103" s="49"/>
+      <c r="H103" s="49"/>
+      <c r="I103" s="49"/>
+      <c r="J103" s="49"/>
+      <c r="K103" s="49"/>
+      <c r="L103" s="49"/>
+      <c r="M103" s="49"/>
+      <c r="N103" s="49"/>
+      <c r="O103" s="49"/>
+      <c r="P103" s="49"/>
+      <c r="Q103" s="49"/>
       <c r="R103" s="6"/>
       <c r="S103" s="14"/>
       <c r="T103" s="14"/>
@@ -4813,24 +4824,24 @@
     </row>
     <row r="107" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
-      <c r="B107" s="47" t="s">
+      <c r="B107" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="C107" s="47"/>
-      <c r="D107" s="47"/>
-      <c r="E107" s="47" t="s">
+      <c r="C107" s="129"/>
+      <c r="D107" s="129"/>
+      <c r="E107" s="129" t="s">
         <v>49</v>
       </c>
-      <c r="F107" s="47"/>
-      <c r="G107" s="47"/>
-      <c r="H107" s="47"/>
-      <c r="I107" s="47"/>
-      <c r="J107" s="47" t="s">
+      <c r="F107" s="129"/>
+      <c r="G107" s="129"/>
+      <c r="H107" s="129"/>
+      <c r="I107" s="129"/>
+      <c r="J107" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="K107" s="47"/>
-      <c r="L107" s="47"/>
-      <c r="M107" s="47"/>
+      <c r="K107" s="129"/>
+      <c r="L107" s="129"/>
+      <c r="M107" s="129"/>
       <c r="N107" s="39" t="s">
         <v>69</v>
       </c>
@@ -4855,24 +4866,24 @@
     </row>
     <row r="108" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
-      <c r="B108" s="49" t="s">
+      <c r="B108" s="130" t="s">
         <v>65</v>
       </c>
-      <c r="C108" s="49"/>
-      <c r="D108" s="49"/>
-      <c r="E108" s="50" t="s">
+      <c r="C108" s="130"/>
+      <c r="D108" s="130"/>
+      <c r="E108" s="131" t="s">
         <v>50</v>
       </c>
-      <c r="F108" s="50"/>
-      <c r="G108" s="50"/>
-      <c r="H108" s="50"/>
-      <c r="I108" s="50"/>
-      <c r="J108" s="51" t="s">
+      <c r="F108" s="131"/>
+      <c r="G108" s="131"/>
+      <c r="H108" s="131"/>
+      <c r="I108" s="131"/>
+      <c r="J108" s="132" t="s">
         <v>54</v>
       </c>
-      <c r="K108" s="51"/>
-      <c r="L108" s="51"/>
-      <c r="M108" s="51"/>
+      <c r="K108" s="132"/>
+      <c r="L108" s="132"/>
+      <c r="M108" s="132"/>
       <c r="N108" s="29"/>
       <c r="O108" s="30"/>
       <c r="P108" s="30"/>
@@ -5165,13 +5176,13 @@
       </c>
       <c r="C117" s="44"/>
       <c r="D117" s="44"/>
-      <c r="E117" s="132" t="s">
+      <c r="E117" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="F117" s="132"/>
-      <c r="G117" s="132"/>
-      <c r="H117" s="132"/>
-      <c r="I117" s="132"/>
+      <c r="F117" s="47"/>
+      <c r="G117" s="47"/>
+      <c r="H117" s="47"/>
+      <c r="I117" s="47"/>
       <c r="J117" s="46" t="s">
         <v>59</v>
       </c>
@@ -5575,25 +5586,115 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="152">
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="E116:I116"/>
-    <mergeCell ref="J116:M116"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="E117:I117"/>
-    <mergeCell ref="J117:M117"/>
-    <mergeCell ref="B118:D118"/>
-    <mergeCell ref="E118:I118"/>
-    <mergeCell ref="J118:M118"/>
-    <mergeCell ref="C103:Q103"/>
-    <mergeCell ref="C93:Q93"/>
-    <mergeCell ref="C98:Q98"/>
-    <mergeCell ref="C68:Q68"/>
-    <mergeCell ref="C69:Q69"/>
-    <mergeCell ref="C83:Q83"/>
-    <mergeCell ref="C73:Q73"/>
-    <mergeCell ref="C74:Q74"/>
-    <mergeCell ref="C78:Q78"/>
-    <mergeCell ref="C79:Q79"/>
+    <mergeCell ref="B119:D119"/>
+    <mergeCell ref="E119:I119"/>
+    <mergeCell ref="J119:M119"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="E107:I107"/>
+    <mergeCell ref="J107:M107"/>
+    <mergeCell ref="B114:D114"/>
+    <mergeCell ref="E114:I114"/>
+    <mergeCell ref="J114:M114"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="E108:I108"/>
+    <mergeCell ref="J108:M108"/>
+    <mergeCell ref="B109:D109"/>
+    <mergeCell ref="E109:I109"/>
+    <mergeCell ref="J109:M109"/>
+    <mergeCell ref="B110:D110"/>
+    <mergeCell ref="E110:I110"/>
+    <mergeCell ref="J110:M110"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="E111:I111"/>
+    <mergeCell ref="J111:M111"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="E112:I112"/>
+    <mergeCell ref="J112:M112"/>
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="E113:I113"/>
+    <mergeCell ref="J113:M113"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="E115:I115"/>
+    <mergeCell ref="J115:M115"/>
+    <mergeCell ref="X92:AA92"/>
+    <mergeCell ref="X93:AA93"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:Q5"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="G8:L8"/>
+    <mergeCell ref="P13:Q14"/>
+    <mergeCell ref="N10:O11"/>
+    <mergeCell ref="P10:Q11"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="J11:L14"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="P7:Q8"/>
+    <mergeCell ref="D62:Q62"/>
+    <mergeCell ref="P23:Q25"/>
+    <mergeCell ref="P26:Q28"/>
+    <mergeCell ref="D60:Q60"/>
+    <mergeCell ref="P29:Q31"/>
+    <mergeCell ref="P32:Q34"/>
+    <mergeCell ref="P35:Q37"/>
+    <mergeCell ref="D46:Q46"/>
+    <mergeCell ref="D47:Q47"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="P51:Q52"/>
+    <mergeCell ref="P53:Q55"/>
+    <mergeCell ref="P56:Q58"/>
+    <mergeCell ref="P38:Q40"/>
+    <mergeCell ref="P41:Q43"/>
+    <mergeCell ref="X91:AA91"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="D26:E28"/>
+    <mergeCell ref="D29:E31"/>
+    <mergeCell ref="D32:E34"/>
+    <mergeCell ref="D35:E37"/>
+    <mergeCell ref="D41:E43"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="D51:O52"/>
+    <mergeCell ref="O41:O43"/>
+    <mergeCell ref="F32:N32"/>
+    <mergeCell ref="F33:N34"/>
+    <mergeCell ref="F35:N35"/>
+    <mergeCell ref="F36:N37"/>
+    <mergeCell ref="F38:N38"/>
+    <mergeCell ref="F39:N40"/>
+    <mergeCell ref="F41:N41"/>
+    <mergeCell ref="F42:N43"/>
+    <mergeCell ref="D45:Q45"/>
+    <mergeCell ref="C88:Q88"/>
+    <mergeCell ref="C89:Q89"/>
+    <mergeCell ref="C84:Q84"/>
+    <mergeCell ref="N13:O14"/>
+    <mergeCell ref="D38:E40"/>
+    <mergeCell ref="F26:N26"/>
+    <mergeCell ref="F27:N28"/>
+    <mergeCell ref="F29:N29"/>
+    <mergeCell ref="F30:N31"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="O26:O28"/>
+    <mergeCell ref="O29:O31"/>
+    <mergeCell ref="O32:O34"/>
+    <mergeCell ref="O35:O37"/>
+    <mergeCell ref="O38:O40"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="B2:P2"/>
     <mergeCell ref="B20:B22"/>
@@ -5618,115 +5719,25 @@
     <mergeCell ref="O23:O25"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="B18:B19"/>
-    <mergeCell ref="N13:O14"/>
-    <mergeCell ref="D38:E40"/>
-    <mergeCell ref="F26:N26"/>
-    <mergeCell ref="F27:N28"/>
-    <mergeCell ref="F29:N29"/>
-    <mergeCell ref="F30:N31"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="O26:O28"/>
-    <mergeCell ref="O29:O31"/>
-    <mergeCell ref="O32:O34"/>
-    <mergeCell ref="O35:O37"/>
-    <mergeCell ref="O38:O40"/>
-    <mergeCell ref="X91:AA91"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="D26:E28"/>
-    <mergeCell ref="D29:E31"/>
-    <mergeCell ref="D32:E34"/>
-    <mergeCell ref="D35:E37"/>
-    <mergeCell ref="D41:E43"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="D51:O52"/>
-    <mergeCell ref="O41:O43"/>
-    <mergeCell ref="F32:N32"/>
-    <mergeCell ref="F33:N34"/>
-    <mergeCell ref="F35:N35"/>
-    <mergeCell ref="F36:N37"/>
-    <mergeCell ref="F38:N38"/>
-    <mergeCell ref="F39:N40"/>
-    <mergeCell ref="F41:N41"/>
-    <mergeCell ref="F42:N43"/>
-    <mergeCell ref="D45:Q45"/>
-    <mergeCell ref="C88:Q88"/>
-    <mergeCell ref="C89:Q89"/>
-    <mergeCell ref="C84:Q84"/>
-    <mergeCell ref="P26:Q28"/>
-    <mergeCell ref="D60:Q60"/>
-    <mergeCell ref="P29:Q31"/>
-    <mergeCell ref="P32:Q34"/>
-    <mergeCell ref="P35:Q37"/>
-    <mergeCell ref="D46:Q46"/>
-    <mergeCell ref="D47:Q47"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="P51:Q52"/>
-    <mergeCell ref="P53:Q55"/>
-    <mergeCell ref="P56:Q58"/>
-    <mergeCell ref="P38:Q40"/>
-    <mergeCell ref="P41:Q43"/>
-    <mergeCell ref="B113:D113"/>
-    <mergeCell ref="E113:I113"/>
-    <mergeCell ref="J113:M113"/>
-    <mergeCell ref="B115:D115"/>
-    <mergeCell ref="E115:I115"/>
-    <mergeCell ref="J115:M115"/>
-    <mergeCell ref="X92:AA92"/>
-    <mergeCell ref="X93:AA93"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:Q5"/>
-    <mergeCell ref="G4:L4"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="G6:L6"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="G8:L8"/>
-    <mergeCell ref="P13:Q14"/>
-    <mergeCell ref="N10:O11"/>
-    <mergeCell ref="P10:Q11"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="J11:L14"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="D62:Q62"/>
-    <mergeCell ref="P23:Q25"/>
-    <mergeCell ref="B119:D119"/>
-    <mergeCell ref="E119:I119"/>
-    <mergeCell ref="J119:M119"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="E107:I107"/>
-    <mergeCell ref="J107:M107"/>
-    <mergeCell ref="B114:D114"/>
-    <mergeCell ref="E114:I114"/>
-    <mergeCell ref="J114:M114"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="E108:I108"/>
-    <mergeCell ref="J108:M108"/>
-    <mergeCell ref="B109:D109"/>
-    <mergeCell ref="E109:I109"/>
-    <mergeCell ref="J109:M109"/>
-    <mergeCell ref="B110:D110"/>
-    <mergeCell ref="E110:I110"/>
-    <mergeCell ref="J110:M110"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="E111:I111"/>
-    <mergeCell ref="J111:M111"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="E112:I112"/>
-    <mergeCell ref="J112:M112"/>
+    <mergeCell ref="C103:Q103"/>
+    <mergeCell ref="C93:Q93"/>
+    <mergeCell ref="C98:Q98"/>
+    <mergeCell ref="C68:Q68"/>
+    <mergeCell ref="C69:Q69"/>
+    <mergeCell ref="C83:Q83"/>
+    <mergeCell ref="C73:Q73"/>
+    <mergeCell ref="C74:Q74"/>
+    <mergeCell ref="C78:Q78"/>
+    <mergeCell ref="C79:Q79"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="E116:I116"/>
+    <mergeCell ref="J116:M116"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="E117:I117"/>
+    <mergeCell ref="J117:M117"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="E118:I118"/>
+    <mergeCell ref="J118:M118"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -5826,6 +5837,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2B826667128664EB5BF996137814269" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fae99688d4eff97766fcbf054e39ddba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cef818d1-7f02-40bd-b635-f979fe7dc7c8" xmlns:ns3="123f82ff-efc3-4fb3-befe-02b68418169f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d2063e240d92a77e1e922105c74daf1d" ns2:_="" ns3:_="">
     <xsd:import namespace="cef818d1-7f02-40bd-b635-f979fe7dc7c8"/>
@@ -6042,15 +6062,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773514D2-8AA7-40BF-BC7F-C770723F6669}">
   <ds:schemaRefs>
@@ -6069,6 +6080,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57E74503-2AD6-4615-B95D-C25393FC43B6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0240A04-A3AB-4903-A7D7-B79D60CC1221}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6085,12 +6104,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57E74503-2AD6-4615-B95D-C25393FC43B6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>